<commit_message>
add vn expire id date
</commit_message>
<xml_diff>
--- a/Data/Output/Tracking.xlsx
+++ b/Data/Output/Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rpa\finalproject\uipath\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D0ACE0-3381-43DA-B904-086BC276E1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5131F15C-104C-48A9-88EF-221088132A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="1116" yWindow="1116" windowWidth="21192" windowHeight="10596" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="768" yWindow="768" windowWidth="21192" windowHeight="10596" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -397,10 +397,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D7"/>
+  <x:dimension ref="A1:D1"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A2" sqref="A2 2:7"/>
+      <x:selection activeCell="A2" sqref="A2 2:5"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,7 +419,7 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -433,7 +433,7 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <x:row r="3" spans="1:4">
       <x:c r="A3" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -447,7 +447,7 @@
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
@@ -459,48 +459,6 @@
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <x:c r="A5" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <x:c r="A6" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <x:c r="A7" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>4</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>